<commit_message>
Refactor admin panel layout and styles; add file upload feature and improve form validation
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -435,9 +435,31 @@
         <v>Trusted</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Anita</v>
+      </c>
+      <c r="B4" t="str">
+        <v>8368547181</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Trusted</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Ayush</v>
+      </c>
+      <c r="B5" t="str">
+        <v>8882292108</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Blacklisted</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update data.xlsx with new content
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -397,13 +397,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>name</v>
+      </c>
+      <c r="B1" t="str">
+        <v>mobile</v>
+      </c>
+      <c r="C1" t="str">
+        <v>status</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>Ayush</v>
+      </c>
+      <c r="B2" t="str">
+        <v>8368547177</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Trusted</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Amaan</v>
+      </c>
+      <c r="B3" t="str">
+        <v>9811714919</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Trusted</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Mummy</v>
+      </c>
+      <c r="B4" t="str">
+        <v>8368547181</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Trusted</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Mummy</v>
+      </c>
+      <c r="B5" t="str">
+        <v>8368547182</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Fraud</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>